<commit_message>
Update Plooto bulk payment import template
</commit_message>
<xml_diff>
--- a/assets/docs/Plooto_Bulkpayment_Import_template.xlsx
+++ b/assets/docs/Plooto_Bulkpayment_Import_template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10921"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59EB3092-0322-4406-B1E9-AB6FA8CE57FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D7DC5A-9513-C349-91BA-8F9E8EA3E6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="99">
   <si>
     <t>Plooto Mass Contact Import</t>
   </si>
@@ -462,39 +462,21 @@
     <t>USD</t>
   </si>
   <si>
-    <t>Amanda</t>
-  </si>
-  <si>
-    <t>Adeeryaj</t>
-  </si>
-  <si>
-    <t>oeric</t>
-  </si>
-  <si>
-    <t>amanda.ntow1@gmail.com</t>
-  </si>
-  <si>
-    <t>adeeryaj@gmail.com</t>
-  </si>
-  <si>
-    <t>oericboateng@gmail.com</t>
-  </si>
-  <si>
-    <t>Who is sending this payment?</t>
-  </si>
-  <si>
-    <t>GSSUBC</t>
-  </si>
-  <si>
     <t>Amount 
 (Required)</t>
+  </si>
+  <si>
+    <t>GSS</t>
+  </si>
+  <si>
+    <t>What is the three-letter acronym of the Graduate Student Society?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -594,15 +576,8 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF242424"/>
       <name val="Aptos Narrow"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -860,7 +835,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
@@ -925,8 +900,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -935,6 +908,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -946,9 +922,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1275,118 +1248,118 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.77734375" style="3"/>
+    <col min="1" max="1" width="30.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36" customHeight="1">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="38"/>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="36"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="O2" s="5"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="O4" s="5"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>3</v>
       </c>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>4</v>
       </c>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>29</v>
       </c>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>7</v>
       </c>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -1422,56 +1395,56 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D45" sqref="D45"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3:G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" style="21" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" style="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.6640625" style="24" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" style="24" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.33203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" style="15" customWidth="1"/>
+    <col min="10" max="10" width="16.5" style="15" customWidth="1"/>
     <col min="11" max="11" width="14.33203125" style="16" customWidth="1"/>
     <col min="12" max="12" width="19.33203125" style="15" customWidth="1"/>
-    <col min="13" max="13" width="13.109375" style="15" customWidth="1"/>
-    <col min="14" max="14" width="30.44140625" style="15" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" style="15" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" style="15" customWidth="1"/>
+    <col min="14" max="14" width="30.5" style="15" customWidth="1"/>
+    <col min="15" max="15" width="11.5" style="15" customWidth="1"/>
     <col min="16" max="16" width="16" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.109375" style="1"/>
+    <col min="17" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="22.8">
-      <c r="B1" s="43" t="s">
+    <row r="1" spans="1:16" ht="24" x14ac:dyDescent="0.2">
+      <c r="B1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="42" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="39" t="s">
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="41"/>
-    </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" ht="55.5" customHeight="1">
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="40"/>
+    </row>
+    <row r="2" spans="1:16" s="2" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>16</v>
@@ -1519,16 +1492,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
-      <c r="B3" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>96</v>
-      </c>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D3" s="33"/>
       <c r="E3" s="23" t="s">
         <v>14</v>
       </c>
@@ -1536,25 +1501,17 @@
         <v>13</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I3" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="B4" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>97</v>
-      </c>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D4" s="33"/>
       <c r="E4" s="23" t="s">
         <v>14</v>
       </c>
@@ -1562,25 +1519,17 @@
         <v>13</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I4" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="B5" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>98</v>
-      </c>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D5" s="33"/>
       <c r="E5" s="23" t="s">
         <v>14</v>
       </c>
@@ -1588,18 +1537,17 @@
         <v>13</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="C6" s="35"/>
-      <c r="D6" s="34"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D6" s="33"/>
       <c r="E6" s="23" t="s">
         <v>14</v>
       </c>
@@ -1607,18 +1555,17 @@
         <v>13</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="C7" s="35"/>
-      <c r="D7" s="34"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D7" s="33"/>
       <c r="E7" s="23" t="s">
         <v>14</v>
       </c>
@@ -1626,18 +1573,17 @@
         <v>13</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I7" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="C8" s="35"/>
-      <c r="D8" s="34"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D8" s="33"/>
       <c r="E8" s="23" t="s">
         <v>14</v>
       </c>
@@ -1645,17 +1591,17 @@
         <v>13</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="D9" s="20"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D9" s="33"/>
       <c r="E9" s="23" t="s">
         <v>14</v>
       </c>
@@ -1663,16 +1609,16 @@
         <v>13</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E10" s="23" t="s">
         <v>14</v>
       </c>
@@ -1680,16 +1626,16 @@
         <v>13</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E11" s="23" t="s">
         <v>14</v>
       </c>
@@ -1697,16 +1643,16 @@
         <v>13</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E12" s="23" t="s">
         <v>14</v>
       </c>
@@ -1714,16 +1660,16 @@
         <v>13</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E13" s="23" t="s">
         <v>14</v>
       </c>
@@ -1731,16 +1677,16 @@
         <v>13</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E14" s="23" t="s">
         <v>14</v>
       </c>
@@ -1748,16 +1694,16 @@
         <v>13</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E15" s="23" t="s">
         <v>14</v>
       </c>
@@ -1765,16 +1711,16 @@
         <v>13</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E16" s="23" t="s">
         <v>14</v>
       </c>
@@ -1782,13 +1728,13 @@
         <v>13</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1799,21 +1745,16 @@
     <mergeCell ref="E1:I1"/>
   </mergeCells>
   <dataValidations xWindow="179" yWindow="385" count="3">
-    <dataValidation type="custom" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Contact email" prompt="Enter valid email" sqref="C9:C1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
-      <formula1>SEARCH(".",C9,(SEARCH("@",C9,1))+2)&gt;0</formula1>
+    <dataValidation type="custom" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Contact email" prompt="Enter valid email" sqref="C3:C1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
+      <formula1>SEARCH(".",C3,(SEARCH("@",C3,1))+2)&gt;0</formula1>
     </dataValidation>
     <dataValidation operator="greaterThan" allowBlank="1" promptTitle="Contact email" prompt="Enter valid email" sqref="D10:D1048576 G3:I1048576" xr:uid="{00000000-0002-0000-0300-000003000000}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Bank Country" error="Please select a country from the provided list" promptTitle="Contact Bank Country" prompt="Please enter Canada or United States" sqref="E17:E1048576" xr:uid="{2C2F750E-405E-C14E-8AB7-D2070B10A6EF}">
       <formula1>"United States,Canada"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="mailto:amanda.ntow1@gmail.com" xr:uid="{679F4186-6C62-4C42-8BAF-7465551801D2}"/>
-    <hyperlink ref="C4" r:id="rId2" display="mailto:adeeryaj@gmail.com" xr:uid="{3B01A1C3-D2ED-413A-8838-DE10312129D7}"/>
-    <hyperlink ref="C5" r:id="rId3" display="mailto:oericboateng@gmail.com" xr:uid="{00036B02-3DBF-4B1A-93FF-62D46B681198}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="179" yWindow="385" count="4">
@@ -1855,13 +1796,13 @@
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>14</v>
       </c>
@@ -1875,7 +1816,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
         <v>32</v>
       </c>
@@ -1892,7 +1833,7 @@
       <c r="H2" s="31"/>
       <c r="I2" s="31"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
         <v>33</v>
       </c>
@@ -1907,7 +1848,7 @@
       <c r="H3" s="32"/>
       <c r="I3" s="32"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
         <v>34</v>
       </c>
@@ -1918,7 +1859,7 @@
       <c r="H4" s="32"/>
       <c r="I4" s="32"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
         <v>35</v>
       </c>
@@ -1929,7 +1870,7 @@
       <c r="H5" s="32"/>
       <c r="I5" s="32"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
         <v>36</v>
       </c>
@@ -1940,7 +1881,7 @@
       <c r="H6" s="32"/>
       <c r="I6" s="32"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
         <v>37</v>
       </c>
@@ -1951,7 +1892,7 @@
       <c r="H7" s="32"/>
       <c r="I7" s="32"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
         <v>38</v>
       </c>
@@ -1962,7 +1903,7 @@
       <c r="H8" s="32"/>
       <c r="I8" s="32"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
         <v>39</v>
       </c>
@@ -1973,7 +1914,7 @@
       <c r="H9" s="32"/>
       <c r="I9" s="32"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>40</v>
       </c>
@@ -1984,7 +1925,7 @@
       <c r="H10" s="32"/>
       <c r="I10" s="32"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
         <v>41</v>
       </c>
@@ -1995,7 +1936,7 @@
       <c r="H11" s="32"/>
       <c r="I11" s="32"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="s">
         <v>42</v>
       </c>
@@ -2006,7 +1947,7 @@
       <c r="H12" s="32"/>
       <c r="I12" s="32"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
         <v>43</v>
       </c>
@@ -2017,7 +1958,7 @@
       <c r="H13" s="32"/>
       <c r="I13" s="32"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
         <v>44</v>
       </c>
@@ -2028,7 +1969,7 @@
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
       <c r="B15" s="28" t="s">
         <v>58</v>
@@ -2037,7 +1978,7 @@
       <c r="H15" s="32"/>
       <c r="I15" s="32"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
       <c r="B16" s="28" t="s">
         <v>59</v>
@@ -2046,7 +1987,7 @@
       <c r="H16" s="32"/>
       <c r="I16" s="32"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="27"/>
       <c r="B17" s="28" t="s">
         <v>60</v>
@@ -2055,7 +1996,7 @@
       <c r="H17" s="32"/>
       <c r="I17" s="32"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="27"/>
       <c r="B18" s="28" t="s">
         <v>61</v>
@@ -2064,7 +2005,7 @@
       <c r="H18" s="32"/>
       <c r="I18" s="32"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="27"/>
       <c r="B19" s="28" t="s">
         <v>62</v>
@@ -2073,7 +2014,7 @@
       <c r="H19" s="32"/>
       <c r="I19" s="32"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="28" t="s">
         <v>63</v>
@@ -2082,7 +2023,7 @@
       <c r="H20" s="32"/>
       <c r="I20" s="32"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="27"/>
       <c r="B21" s="28" t="s">
         <v>64</v>
@@ -2091,7 +2032,7 @@
       <c r="H21" s="32"/>
       <c r="I21" s="32"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="27"/>
       <c r="B22" s="28" t="s">
         <v>65</v>
@@ -2100,7 +2041,7 @@
       <c r="H22" s="32"/>
       <c r="I22" s="32"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="28" t="s">
         <v>66</v>
@@ -2109,7 +2050,7 @@
       <c r="H23" s="32"/>
       <c r="I23" s="32"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
       <c r="B24" s="28" t="s">
         <v>67</v>
@@ -2118,7 +2059,7 @@
       <c r="H24" s="32"/>
       <c r="I24" s="32"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="28" t="s">
         <v>68</v>
@@ -2127,7 +2068,7 @@
       <c r="H25" s="32"/>
       <c r="I25" s="32"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
       <c r="B26" s="28" t="s">
         <v>69</v>
@@ -2136,7 +2077,7 @@
       <c r="H26" s="32"/>
       <c r="I26" s="32"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
       <c r="B27" s="28" t="s">
         <v>70</v>
@@ -2145,7 +2086,7 @@
       <c r="H27" s="32"/>
       <c r="I27" s="32"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
       <c r="B28" s="28" t="s">
         <v>71</v>
@@ -2154,7 +2095,7 @@
       <c r="H28" s="32"/>
       <c r="I28" s="32"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="27"/>
       <c r="B29" s="28" t="s">
         <v>72</v>
@@ -2163,7 +2104,7 @@
       <c r="H29" s="32"/>
       <c r="I29" s="32"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="27"/>
       <c r="B30" s="28" t="s">
         <v>73</v>
@@ -2172,7 +2113,7 @@
       <c r="H30" s="32"/>
       <c r="I30" s="32"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="27"/>
       <c r="B31" s="28" t="s">
         <v>74</v>
@@ -2181,7 +2122,7 @@
       <c r="H31" s="32"/>
       <c r="I31" s="32"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
       <c r="B32" s="28" t="s">
         <v>75</v>
@@ -2190,7 +2131,7 @@
       <c r="H32" s="32"/>
       <c r="I32" s="32"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="27"/>
       <c r="B33" s="28" t="s">
         <v>76</v>
@@ -2199,7 +2140,7 @@
       <c r="H33" s="32"/>
       <c r="I33" s="32"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="27"/>
       <c r="B34" s="28" t="s">
         <v>77</v>
@@ -2208,7 +2149,7 @@
       <c r="H34" s="32"/>
       <c r="I34" s="32"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="27"/>
       <c r="B35" s="28" t="s">
         <v>78</v>
@@ -2217,7 +2158,7 @@
       <c r="H35" s="32"/>
       <c r="I35" s="32"/>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="27"/>
       <c r="B36" s="28" t="s">
         <v>79</v>
@@ -2226,7 +2167,7 @@
       <c r="H36" s="32"/>
       <c r="I36" s="32"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="27"/>
       <c r="B37" s="28" t="s">
         <v>80</v>
@@ -2235,7 +2176,7 @@
       <c r="H37" s="32"/>
       <c r="I37" s="32"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="27"/>
       <c r="B38" s="28" t="s">
         <v>81</v>
@@ -2244,7 +2185,7 @@
       <c r="H38" s="32"/>
       <c r="I38" s="32"/>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="27"/>
       <c r="B39" s="28" t="s">
         <v>82</v>
@@ -2253,7 +2194,7 @@
       <c r="H39" s="32"/>
       <c r="I39" s="32"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="27"/>
       <c r="B40" s="28" t="s">
         <v>83</v>
@@ -2262,7 +2203,7 @@
       <c r="H40" s="32"/>
       <c r="I40" s="32"/>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="27"/>
       <c r="B41" s="28" t="s">
         <v>84</v>
@@ -2271,7 +2212,7 @@
       <c r="H41" s="32"/>
       <c r="I41" s="32"/>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="27"/>
       <c r="B42" s="28" t="s">
         <v>85</v>
@@ -2280,7 +2221,7 @@
       <c r="H42" s="32"/>
       <c r="I42" s="32"/>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="27"/>
       <c r="B43" s="28" t="s">
         <v>86</v>
@@ -2289,7 +2230,7 @@
       <c r="H43" s="32"/>
       <c r="I43" s="32"/>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="27"/>
       <c r="B44" s="28" t="s">
         <v>87</v>
@@ -2298,7 +2239,7 @@
       <c r="H44" s="32"/>
       <c r="I44" s="32"/>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="27"/>
       <c r="B45" s="28" t="s">
         <v>88</v>
@@ -2307,7 +2248,7 @@
       <c r="H45" s="32"/>
       <c r="I45" s="32"/>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="27"/>
       <c r="B46" s="28" t="s">
         <v>89</v>
@@ -2316,7 +2257,7 @@
       <c r="H46" s="32"/>
       <c r="I46" s="32"/>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="27"/>
       <c r="B47" s="28" t="s">
         <v>90</v>
@@ -2325,7 +2266,7 @@
       <c r="H47" s="32"/>
       <c r="I47" s="32"/>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="27"/>
       <c r="B48" s="28" t="s">
         <v>91</v>
@@ -2334,7 +2275,7 @@
       <c r="H48" s="32"/>
       <c r="I48" s="32"/>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="27"/>
       <c r="B49" s="28" t="s">
         <v>92</v>
@@ -2343,7 +2284,7 @@
       <c r="H49" s="32"/>
       <c r="I49" s="32"/>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="27"/>
       <c r="B50" s="28" t="s">
         <v>93</v>
@@ -2352,7 +2293,7 @@
       <c r="H50" s="32"/>
       <c r="I50" s="32"/>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="27"/>
       <c r="B51" s="28" t="s">
         <v>94</v>

</xml_diff>